<commit_message>
convert syst_tot to absolute value. added e06009_rd.
</commit_message>
<xml_diff>
--- a/data/JAM/10035.xlsx
+++ b/data/JAM/10035.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,35 +20,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="27">
   <si>
     <t xml:space="preserve">exp</t>
   </si>
   <si>
+    <t xml:space="preserve">length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsilon</t>
+  </si>
+  <si>
     <t xml:space="preserve">target</t>
   </si>
   <si>
-    <t xml:space="preserve">length </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">theta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsilon</t>
-  </si>
-  <si>
     <t xml:space="preserve">current</t>
   </si>
   <si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">e140x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2</t>
   </si>
   <si>
     <t xml:space="preserve">4cm</t>
@@ -237,19 +234,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="14" min="1" style="1" width="13.0510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="15" style="2" width="13.0510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.0510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="13.0510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="1" style="1" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="14" style="2" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1023" min="20" style="1" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.8571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,39 +279,36 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -324,61 +319,58 @@
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
+      <c r="C2" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.5</v>
+        <v>3.3</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>3.3</v>
+        <v>0.636</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.636</v>
+        <v>28.261</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>28.261</v>
-      </c>
-      <c r="I2" s="1" t="n">
         <v>0.342</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
+      <c r="L2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0.280446108357514</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0.280446108357514</v>
+        <v>3.53618516529212</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>3.53618516529212</v>
+        <v>0.692026780279976</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>0.692026780279976</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2" t="n">
         <v>0.310160132525621</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="T2" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -389,61 +381,58 @@
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
+      <c r="C3" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>4</v>
+        <v>1.336</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>1.336</v>
+        <v>17.598</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>17.598</v>
-      </c>
-      <c r="I3" s="1" t="n">
         <v>0.579</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>26</v>
+      <c r="L3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0.284934601867872</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>0.284934601867872</v>
+        <v>2.05974966973846</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>2.05974966973846</v>
+        <v>0.707451224574512</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>0.707451224574512</v>
-      </c>
-      <c r="R3" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="2" t="n">
         <v>0.310160132525621</v>
       </c>
-      <c r="U3" s="1" t="n">
+      <c r="T3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -454,61 +443,58 @@
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
+      <c r="C4" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>0.5</v>
+        <v>4.95</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>4.95</v>
+        <v>2.286</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>2.286</v>
+        <v>12.067</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>12.067</v>
-      </c>
-      <c r="I4" s="1" t="n">
         <v>0.746</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>26</v>
+      <c r="L4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0.282106905348453</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0.282106905348453</v>
+        <v>1.23539813061332</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>1.23539813061332</v>
+        <v>0.740498034076016</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0.740498034076016</v>
-      </c>
-      <c r="R4" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2" t="n">
         <v>0.310160132525621</v>
       </c>
-      <c r="U4" s="1" t="n">
+      <c r="T4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -519,61 +505,58 @@
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
+      <c r="C5" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>1</v>
+        <v>6.45</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>6.45</v>
+        <v>1.121</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>1.121</v>
+        <v>21.432</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>21.432</v>
-      </c>
-      <c r="I5" s="1" t="n">
         <v>0.322</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
+      <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0.333812036554548</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>0.333812036554548</v>
+        <v>2.42534754990566</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>2.42534754990566</v>
+        <v>0.75990099009901</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>0.75990099009901</v>
-      </c>
-      <c r="R5" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="2" t="n">
         <v>0.348619688007481</v>
       </c>
-      <c r="U5" s="1" t="n">
+      <c r="T5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -584,61 +567,58 @@
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
+      <c r="C6" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>6.9</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>6.9</v>
+        <v>1.571</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1.571</v>
+        <v>17.47</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>17.47</v>
-      </c>
-      <c r="I6" s="1" t="n">
         <v>0.419</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>26</v>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0.333089323825153</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>0.333089323825153</v>
+        <v>2.43383295135142</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>2.43383295135142</v>
+        <v>0.70106341079165</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>0.70106341079165</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="2" t="n">
         <v>0.348619688007481</v>
       </c>
-      <c r="U6" s="1" t="n">
+      <c r="T6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -649,61 +629,58 @@
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
+      <c r="C7" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>1</v>
+        <v>7.99</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>7.99</v>
+        <v>2.661</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>2.661</v>
+        <v>12.45</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>12.45</v>
-      </c>
-      <c r="I7" s="1" t="n">
         <v>0.588</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>26</v>
+      <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0.339748001466008</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>0.339748001466008</v>
+        <v>1.38248957675937</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>1.38248957675937</v>
+        <v>0.718933333333333</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>0.718933333333333</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="2" t="n">
         <v>0.348619688007481</v>
       </c>
-      <c r="U7" s="1" t="n">
+      <c r="T7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -712,63 +689,60 @@
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.35</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>3</v>
+        <v>5.6</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>5.6</v>
+        <v>1.032</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>1.032</v>
+        <v>42.223</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>42.223</v>
-      </c>
-      <c r="I8" s="1" t="n">
         <v>0.297</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>26</v>
+      <c r="L8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0.276933377920377</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>0.276933377920377</v>
+        <v>2.15912191976053</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>2.15912191976053</v>
+        <v>0.705276705276705</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>0.705276705276705</v>
-      </c>
-      <c r="R8" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" s="2" t="n">
         <v>0.186797005789584</v>
       </c>
-      <c r="U8" s="1" t="n">
+      <c r="T8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -777,63 +751,60 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.35</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>3</v>
+        <v>6.45</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>6.45</v>
+        <v>1.882</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>1.882</v>
+        <v>28.783</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>28.783</v>
-      </c>
-      <c r="I9" s="1" t="n">
         <v>0.488</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>26</v>
+      <c r="L9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0.270880681981136</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>0.270880681981136</v>
+        <v>1.48689002073143</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>1.48689002073143</v>
+        <v>0.715371127995324</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>0.715371127995324</v>
-      </c>
-      <c r="R9" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T9" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" s="2" t="n">
         <v>0.186797005789584</v>
       </c>
-      <c r="U9" s="1" t="n">
+      <c r="T9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -842,63 +813,60 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0.35</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>3</v>
+        <v>7.99</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>7.99</v>
+        <v>3.422</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>3.422</v>
+        <v>19.066</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>19.066</v>
-      </c>
-      <c r="I10" s="1" t="n">
         <v>0.69</v>
       </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>26</v>
+      <c r="L10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0.274458457855615</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>0.274458457855615</v>
+        <v>0.948090840252316</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>0.948090840252316</v>
+        <v>0.729937916762474</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>0.729937916762474</v>
-      </c>
-      <c r="R10" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T10" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="2" t="n">
         <v>0.186797005789584</v>
       </c>
-      <c r="U10" s="1" t="n">
+      <c r="T10" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -907,63 +875,60 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.35</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>3</v>
+        <v>9.75</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>9.75</v>
+        <v>5.182</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>5.182</v>
+        <v>13.996</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>13.996</v>
-      </c>
-      <c r="I11" s="1" t="n">
         <v>0.807</v>
       </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>26</v>
+      <c r="L11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0.274883414124669</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>0.274883414124669</v>
+        <v>0.820639395836031</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>0.820639395836031</v>
+        <v>0.751841359773371</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>0.751841359773371</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T11" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" s="2" t="n">
         <v>0.186797005789584</v>
       </c>
-      <c r="U11" s="1" t="n">
+      <c r="T11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -972,63 +937,60 @@
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0.5</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>3.6</v>
+        <v>4.95</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>4.95</v>
+        <v>1.113</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>1.113</v>
+        <v>47.675</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>47.675</v>
-      </c>
-      <c r="I12" s="1" t="n">
         <v>0.335</v>
       </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>26</v>
+      <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>0.169645869193764</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>0.169645869193764</v>
+        <v>2.14400094772445</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>2.14400094772445</v>
+        <v>0.81072278592008</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>0.81072278592008</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="2" t="n">
         <v>0.155488360308516</v>
       </c>
-      <c r="U12" s="1" t="n">
+      <c r="T12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1037,63 +999,60 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.5</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>3.6</v>
+        <v>5.6</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>5.6</v>
+        <v>1.763</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>1.763</v>
+        <v>35.145</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>35.145</v>
-      </c>
-      <c r="I13" s="1" t="n">
         <v>0.495</v>
       </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>26</v>
+      <c r="L13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0.16887487764501</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>0.16887487764501</v>
+        <v>1.45064295486331</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>1.45064295486331</v>
+        <v>0.757333333333333</v>
       </c>
       <c r="Q13" s="2" t="n">
-        <v>0.757333333333333</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="2" t="n">
         <v>0.155488360308516</v>
       </c>
-      <c r="U13" s="1" t="n">
+      <c r="T13" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1102,63 +1061,60 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0.5</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>3.6</v>
+        <v>6.45</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>6.45</v>
+        <v>2.613</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>2.613</v>
+        <v>26.721</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>26.721</v>
-      </c>
-      <c r="I14" s="1" t="n">
         <v>0.635</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>26</v>
+      <c r="L14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0.172244372495688</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>0.172244372495688</v>
+        <v>0.991701352857101</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>0.991701352857101</v>
+        <v>0.824586628324946</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>0.824586628324946</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T14" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="2" t="n">
         <v>0.155488360308516</v>
       </c>
-      <c r="U14" s="1" t="n">
+      <c r="T14" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1167,63 +1123,60 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0.5</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>3.6</v>
+        <v>6.9</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>6.9</v>
+        <v>3.063</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>3.063</v>
+        <v>23.817</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>23.817</v>
-      </c>
-      <c r="I15" s="1" t="n">
         <v>0.688</v>
       </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>26</v>
+      <c r="L15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0.166649709713687</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>0.166649709713687</v>
+        <v>1.28030002345502</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>1.28030002345502</v>
+        <v>0.794134560092007</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>0.794134560092007</v>
-      </c>
-      <c r="R15" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T15" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" s="2" t="n">
         <v>0.155488360308516</v>
       </c>
-      <c r="U15" s="1" t="n">
+      <c r="T15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1232,63 +1185,60 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0.5</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>3.6</v>
+        <v>9.75</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>9.75</v>
+        <v>5.913</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>5.913</v>
+        <v>14.355</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>14.355</v>
-      </c>
-      <c r="I16" s="1" t="n">
         <v>0.861</v>
       </c>
+      <c r="I16" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>26</v>
+      <c r="L16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0.171787394453965</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>0.171787394453965</v>
+        <v>0.68531906514896</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0.68531906514896</v>
+        <v>0.8256</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>0.8256</v>
-      </c>
-      <c r="R16" s="2" t="n">
-        <v>1.73205080756888</v>
-      </c>
-      <c r="S16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T16" s="2" t="n">
+        <v>1.73205080756888</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" s="2" t="n">
         <v>0.155488360308516</v>
       </c>
-      <c r="U16" s="1" t="n">
+      <c r="T16" s="1" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. separate syst and stat errors in several experients. 2. the R model uncertainty is changed from 2% (simona's paper) from 0.7% (Christy).
</commit_message>
<xml_diff>
--- a/data/JAM/10035.xlsx
+++ b/data/JAM/10035.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">r1998</t>
   </si>
   <si>
-    <t xml:space="preserve">%dR_c</t>
+    <t xml:space="preserve">%dR_u</t>
   </si>
   <si>
     <t xml:space="preserve">e140x</t>
@@ -237,17 +237,17 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="13" min="1" style="1" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="14" style="2" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1023" min="20" style="1" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="17" min="14" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1023" min="20" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,7 +371,7 @@
         <v>0.310160132525621</v>
       </c>
       <c r="T2" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,7 +433,7 @@
         <v>0.310160132525621</v>
       </c>
       <c r="T3" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +495,7 @@
         <v>0.310160132525621</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,7 +557,7 @@
         <v>0.348619688007481</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +619,7 @@
         <v>0.348619688007481</v>
       </c>
       <c r="T6" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,7 +681,7 @@
         <v>0.348619688007481</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +743,7 @@
         <v>0.186797005789584</v>
       </c>
       <c r="T8" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,7 +805,7 @@
         <v>0.186797005789584</v>
       </c>
       <c r="T9" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,7 +867,7 @@
         <v>0.186797005789584</v>
       </c>
       <c r="T10" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,7 +929,7 @@
         <v>0.186797005789584</v>
       </c>
       <c r="T11" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +991,7 @@
         <v>0.155488360308516</v>
       </c>
       <c r="T12" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,7 +1053,7 @@
         <v>0.155488360308516</v>
       </c>
       <c r="T13" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,7 +1115,7 @@
         <v>0.155488360308516</v>
       </c>
       <c r="T14" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,7 +1177,7 @@
         <v>0.155488360308516</v>
       </c>
       <c r="T15" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1239,7 @@
         <v>0.155488360308516</v>
       </c>
       <c r="T16" s="1" t="n">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>